<commit_message>
Edit Wiring plan and add Eagle schematic file
</commit_message>
<xml_diff>
--- a/electrical/wiring_plan.xlsx
+++ b/electrical/wiring_plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT SIBER\PID_motor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Penelitian\GitHub\motor-control-demo-kit\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10854B3-2E27-4995-AF9E-174D271872DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B070DB-8E48-4DB5-91C0-1EF512D0CC5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{15E3AD4C-735A-41DF-B4F0-06194256736E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{15E3AD4C-735A-41DF-B4F0-06194256736E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Arduino Nano</t>
   </si>
@@ -88,6 +88,54 @@
   </si>
   <si>
     <t>D5</t>
+  </si>
+  <si>
+    <t>LCD 16x2 I2C</t>
+  </si>
+  <si>
+    <t>LCD_pwr</t>
+  </si>
+  <si>
+    <t>LCD_gnd</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>LCD_SDA</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>LCD_SCL</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>Pot_5v</t>
+  </si>
+  <si>
+    <t>Pot_GND</t>
+  </si>
+  <si>
+    <t>Pot_output</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>Btn_GND</t>
+  </si>
+  <si>
+    <t>Btn_input</t>
   </si>
 </sst>
 </file>
@@ -125,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -148,17 +196,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -178,7 +257,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -474,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80929BFD-9FEA-41E0-9482-86B5A540704F}">
-  <dimension ref="C1:F11"/>
+  <dimension ref="C1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,125 +565,229 @@
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="G2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
+      <c r="G5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
+      <c r="F9" s="1"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
+      <c r="F14" s="1"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>